<commit_message>
upgraded all files below 0.7.1 to the latest version
</commit_message>
<xml_diff>
--- a/test/core/excel/SingleSheet.xlsx
+++ b/test/core/excel/SingleSheet.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t_laksr\Desktop\DynamoSrc\Dynamo\test\core\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="720" yWindow="405" windowWidth="27555" windowHeight="14085"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="37" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="38" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -55,6 +60,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -103,7 +111,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -136,9 +144,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -171,6 +196,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -347,11 +389,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B6"/>
+  <dimension ref="B2:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -370,16 +410,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>